<commit_message>
Đọc RSS VNExpress and TuoiTre
</commit_message>
<xml_diff>
--- a/me-docs/sum.xlsx
+++ b/me-docs/sum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F918DB-51A5-4BB1-BC07-BAFB7C1D7313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE59FD3A-1E8D-4DEF-BF18-5442891FED60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="MethodNotAllowedHttpException" sheetId="8" r:id="rId7"/>
     <sheet name="check login" sheetId="9" r:id="rId8"/>
     <sheet name="Github Fixed using Token" sheetId="10" r:id="rId9"/>
+    <sheet name="dd vs print_r function" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>config\zvn.php</t>
   </si>
@@ -117,6 +118,18 @@
   </si>
   <si>
     <t>paste Personal access tokens</t>
+  </si>
+  <si>
+    <t>dd($data)</t>
+  </si>
+  <si>
+    <t>echo "&lt;pre&gt;";</t>
+  </si>
+  <si>
+    <t>print_r($data);</t>
+  </si>
+  <si>
+    <t>echo "&lt;/pre&gt;";</t>
   </si>
 </sst>
 </file>
@@ -1999,6 +2012,99 @@
         <a:xfrm>
           <a:off x="609600" y="52387500"/>
           <a:ext cx="3085714" cy="1723810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>48074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{748076D3-44A7-E9A4-2F4F-671F63DABD5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="11258550" cy="1762574"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>8228</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>8809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BA04309-2693-4B74-AB07-8B9EC0308360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2857500"/>
+          <a:ext cx="10371428" cy="5723809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2307,6 +2413,42 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{917D685D-3170-4E8C-994A-304163415E66}">
+  <dimension ref="A2:A15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C979D8D9-5A43-44DD-83F8-870E44A2DD09}">
   <dimension ref="A2:B3"/>
@@ -2570,7 +2712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2E3908-EEEE-4959-B174-2154B06BEA03}">
   <dimension ref="H255:I281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+    <sheetView topLeftCell="A262" workbookViewId="0">
       <selection activeCell="L274" sqref="L274"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajax hiển thị bảng giá vàng và giá coin
</commit_message>
<xml_diff>
--- a/me-docs/sum.xlsx
+++ b/me-docs/sum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C26D115-D1C6-4CA0-A038-F3AC944E6451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355AE627-089A-4D7C-9D39-8F8461B5FA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,9 +133,6 @@
     <t>echo "&lt;/pre&gt;";</t>
   </si>
   <si>
-    <t>git config core.autocrlf false</t>
-  </si>
-  <si>
     <t>Check config</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Config off</t>
+  </si>
+  <si>
+    <t>git config --global core.autocrlf false</t>
   </si>
 </sst>
 </file>
@@ -2179,50 +2179,6 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>18438</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180833</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E6264CC-5542-554B-6921-65FD178A4477}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="2476500"/>
-          <a:ext cx="4895238" cy="1133333"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2246,7 +2202,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2255,6 +2211,50 @@
         <a:xfrm>
           <a:off x="609600" y="4191000"/>
           <a:ext cx="4809524" cy="476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104152</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B37944EA-4223-66CF-8CE6-C40F57755906}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2476500"/>
+          <a:ext cx="4980952" cy="1152381"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2603,30 +2603,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6319D3D3-9E5F-42E8-A56E-5FFD7E4E20F6}">
   <dimension ref="A12:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>